<commit_message>
update and add python3 scripts
</commit_message>
<xml_diff>
--- a/Python3-ThirdPartyLibrary/Chapter07_Excel_openpyxl_Test.xlsx
+++ b/Python3-ThirdPartyLibrary/Chapter07_Excel_openpyxl_Test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9375" windowWidth="24000" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9375" windowWidth="24000" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet-One" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>aaa</t>
   </si>
@@ -31,6 +31,15 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>This is a test!</t>
+  </si>
+  <si>
+    <t>aaa bbb ccc</t>
+  </si>
+  <si>
+    <t>1234567890</t>
   </si>
 </sst>
 </file>
@@ -375,7 +384,7 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -429,7 +438,7 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -483,15 +492,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>